<commit_message>
Put together BoM for the masthead light
</commit_message>
<xml_diff>
--- a/Combiner/BatteryChargerCombinerBoM.xlsx
+++ b/Combiner/BatteryChargerCombinerBoM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BatteryChargerCombinerBoM" sheetId="1" r:id="rId1"/>
@@ -708,7 +708,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1554,12 +1554,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="F2" sqref="F2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,7 +1672,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1728,7 +1727,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>17</v>
       </c>
@@ -1754,7 +1753,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15</v>
       </c>
@@ -1919,7 +1918,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1974,7 +1973,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -2000,7 +1999,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
@@ -2345,7 +2344,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
@@ -3108,105 +3107,54 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I55">
-    <filterColumn colId="6">
-      <filters blank="1">
-        <filter val="06035A220JAT2A"/>
-        <filter val="1264EY-100M=P3"/>
-        <filter val="150060BS75000"/>
-        <filter val="150060GS75000"/>
-        <filter val="150060RS75000"/>
-        <filter val="173950378"/>
-        <filter val="173950578"/>
-        <filter val="705450003"/>
-        <filter val="705450049"/>
-        <filter val="705450072"/>
-        <filter val="BAT750-TP"/>
-        <filter val="BQ24650RVAT"/>
-        <filter val="BQ28Z610DRZT"/>
-        <filter val="CC1210KKX5R9BB475"/>
-        <filter val="CC1210ZKY5VGBB106"/>
-        <filter val="CL10A225KL8NNNC"/>
-        <filter val="CL10B471KB8NNNC"/>
-        <filter val="DMN6040SSD-13"/>
-        <filter val="DMP3099L-7"/>
-        <filter val="DMP4047SSD-13"/>
-        <filter val="ED4164-63-ND"/>
-        <filter val="LMV358SG-13"/>
-        <filter val="MBR0580S1-7"/>
-        <filter val="MC74VHC1G07DTT1G"/>
-        <filter val="MIC5219-3.3YM5-TR"/>
-        <filter val="NTR5103NT1G"/>
-        <filter val="PA2512FKF070R002E"/>
-        <filter val="PE2512FKE070R04L"/>
-        <filter val="PMEG4020ETP,115"/>
-        <filter val="RC0603FR-07100RL"/>
-        <filter val="RC0603FR-0710ML"/>
-        <filter val="RC0603FR-0710RL"/>
-        <filter val="RC0603FR-0715KL"/>
-        <filter val="RC0603FR-07232KL"/>
-        <filter val="RC0603FR-07300KL"/>
-        <filter val="RC0603FR-075K1L"/>
-        <filter val="RC0603FR-0775KL"/>
-        <filter val="RC1206FR-0710RL"/>
-        <filter val="RMCF0603FT2R00"/>
-        <filter val="RMCF0603FT4R99"/>
-        <filter val="S2B-XH-A(LF)(SN)"/>
-        <filter val="S3B-XH-SM4-TB(LF)(SN)"/>
-        <filter val="SN74LVC1G06DBVR"/>
-        <filter val="STWD100NYWY3F"/>
-        <filter val="TCA9543ADR"/>
-        <filter val="TS7211AILT"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I55" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="https://www.digikey.com/product-detail/en/diodes-incorporated/MBR0580S1-7/MBR0580S1-7DICT-ND/5080371"/>
-    <hyperlink ref="G3" r:id="rId2" display="https://www.digikey.com/product-detail/en/micro-commercial-co/BAT750-TP/BAT750-TPMSCT-ND/7681652"/>
-    <hyperlink ref="G13" r:id="rId3" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/1264EY-100M=P3/490-10814-1-ND/5271556"/>
-    <hyperlink ref="G18" r:id="rId4" display="https://www.digikey.com/product-detail/en/on-semiconductor/NTR5103NT1G/NTR5103NT1GOSCT-ND/5801875"/>
-    <hyperlink ref="G26" r:id="rId5" display="https://www.digikey.com/product-detail/en/diodes-incorporated/DMP3099L-7/DMP3099L-7DICT-ND/5218217"/>
-    <hyperlink ref="G22" r:id="rId6" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/S3B-XH-SM4-TB-LF-SN/455-2263-1-ND/1651061"/>
-    <hyperlink ref="G33" r:id="rId7" display="https://www.digikey.com/product-detail/en/on-semiconductor/MC74VHC1G07DTT1G/MC74VHC1G07DTT1GOSCT-ND/1967117"/>
-    <hyperlink ref="G34" r:id="rId8" display="https://www.digikey.com/product-detail/en/texas-instruments/SN74LVC1G06DBVR/296-8483-1-ND/377451"/>
-    <hyperlink ref="G37" r:id="rId9" display="https://www.digikey.com/product-detail/en/texas-instruments/BQ24650RVAT/296-27699-1-ND/2352706"/>
-    <hyperlink ref="G38" r:id="rId10" display="https://www.digikey.com/product-detail/en/texas-instruments/BQ28Z610DRZT/296-43394-1-ND/5813465"/>
-    <hyperlink ref="G39" r:id="rId11" display="https://www.digikey.com/product-detail/en/diodes-incorporated/DMN6040SSD-13/DMN6040SSD-13DICT-ND/3481122"/>
-    <hyperlink ref="G40" r:id="rId12" display="https://www.digikey.com/product-detail/en/diodes-incorporated/DMP4047SSD-13/DMP4047SSD-13DICT-ND/5147416"/>
-    <hyperlink ref="G43" r:id="rId13" display="https://www.digikey.com/product-detail/en/molex-llc/0705450072/WM14782-ND/3302409"/>
-    <hyperlink ref="G44" r:id="rId14" display="https://www.digikey.com/product-detail/en/molex-connector-corporation/0705450003/WM4186-ND/455677"/>
-    <hyperlink ref="G42" r:id="rId15" display="https://www.digikey.com/product-detail/en/molex-connector-corporation/0705450049/WM14780-ND/3302397"/>
-    <hyperlink ref="G45" r:id="rId16" display="https://www.digikey.com/product-detail/en/diodes-incorporated/LMV358SG-13/LMV358SG-13DICT-ND/2182572"/>
-    <hyperlink ref="G46" r:id="rId17" display="https://www.digikey.com/product-detail/en/microchip-technology/MIC5219-3.3YM5-TR/576-1281-1-ND/771902"/>
-    <hyperlink ref="G47" r:id="rId18" display="https://www.digikey.com/product-detail/en/mill-max-manufacturing-corp/310-43-163-41-105000/ED4164-63-ND/4455145"/>
-    <hyperlink ref="G48" r:id="rId19" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/S2B-XH-A-LF-SN/455-2257-ND/1651055"/>
-    <hyperlink ref="G50" r:id="rId20" display="https://www.digikey.com/product-detail/en/nexperia-usa-inc/PMEG4020ETP115/1727-1730-1-ND/4581267"/>
-    <hyperlink ref="G51" r:id="rId21" display="https://www.digikey.com/product-detail/en/stmicroelectronics/STWD100NYWY3F/497-10058-1-ND/2175107"/>
-    <hyperlink ref="G52" r:id="rId22" display="https://www.digikey.com/product-detail/en/texas-instruments/TCA9543ADR/296-42064-1-ND/5246241"/>
-    <hyperlink ref="G53" r:id="rId23" display="https://www.digikey.com/product-detail/en/stmicroelectronics/TS7211AILT/497-3046-1-ND/634884"/>
-    <hyperlink ref="G55" r:id="rId24" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/173950378/732-8242-5-ND/5725366"/>
-    <hyperlink ref="G54" r:id="rId25" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/173950578/732-8243-5-ND/5725367"/>
-    <hyperlink ref="G6" r:id="rId26" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-07100RL/311-100HRCT-ND/729835"/>
-    <hyperlink ref="G9" r:id="rId27" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-0710ML/311-10.0MHRCT-ND/729828"/>
-    <hyperlink ref="G10" r:id="rId28" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-0710RL/311-10.0HRCT-ND/729826"/>
-    <hyperlink ref="G15" r:id="rId29" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-0715KL/311-15.0KHRCT-ND/729900"/>
-    <hyperlink ref="G20" r:id="rId30" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-07232KL/311-232KHRCT-ND/730019"/>
-    <hyperlink ref="G21" r:id="rId31" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RMCF0603FT2R00/RMCF0603FT2R00CT-ND/6053160"/>
-    <hyperlink ref="G25" r:id="rId32" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-07300KL/311-300KHRCT-ND/730092"/>
-    <hyperlink ref="G31" r:id="rId33" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-075K1L/311-5.10KHRCT-ND/730215"/>
-    <hyperlink ref="G32" r:id="rId34" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RMCF0603FT4R99/RMCF0603FT4R99CT-ND/2418080"/>
-    <hyperlink ref="G35" r:id="rId35" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-0775KL/311-75.0KHRCT-ND/730325"/>
-    <hyperlink ref="G11" r:id="rId36" display="https://www.digikey.com/product-detail/en/yageo/RC1206FR-0710RL/311-10.0FRCT-ND/731429"/>
-    <hyperlink ref="G27" r:id="rId37" display="https://www.digikey.com/product-detail/en/yageo/PE2512FKE070R04L/YAG2155CT-ND/5139603"/>
-    <hyperlink ref="G23" r:id="rId38" display="https://www.digikey.com/product-detail/en/yageo/PA2512FKF070R002E/YAG2137CT-ND/5139585"/>
-    <hyperlink ref="G30" r:id="rId39" display="https://www.digikey.com/product-detail/en/yageo/CC1210KKX5R9BB475/311-3533-1-ND/7164554"/>
-    <hyperlink ref="G12" r:id="rId40" display="https://www.digikey.com/product-detail/en/yageo/CC1210ZKY5VGBB106/311-3546-1-ND/7164567"/>
-    <hyperlink ref="G28" r:id="rId41" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10B471KB8NNNC/1276-1094-1-ND/3889180"/>
-    <hyperlink ref="G19" r:id="rId42" display="https://www.digikey.com/product-detail/en/avx-corporation/06035A220JAT2A/478-1167-1-ND/564199"/>
-    <hyperlink ref="G24" r:id="rId43" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10A225KL8NNNC/1276-6726-1-ND/5961585"/>
-    <hyperlink ref="G41" r:id="rId44" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150060GS75000/732-4971-1-ND/4489896"/>
-    <hyperlink ref="G49" r:id="rId45" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150060RS75000/732-4978-1-ND/4489899"/>
-    <hyperlink ref="G36" r:id="rId46" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150060BS75000/732-4966-1-ND/4489893"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://www.digikey.com/product-detail/en/diodes-incorporated/MBR0580S1-7/MBR0580S1-7DICT-ND/5080371" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://www.digikey.com/product-detail/en/micro-commercial-co/BAT750-TP/BAT750-TPMSCT-ND/7681652" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G13" r:id="rId3" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/1264EY-100M=P3/490-10814-1-ND/5271556" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G18" r:id="rId4" display="https://www.digikey.com/product-detail/en/on-semiconductor/NTR5103NT1G/NTR5103NT1GOSCT-ND/5801875" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G26" r:id="rId5" display="https://www.digikey.com/product-detail/en/diodes-incorporated/DMP3099L-7/DMP3099L-7DICT-ND/5218217" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G22" r:id="rId6" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/S3B-XH-SM4-TB-LF-SN/455-2263-1-ND/1651061" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G33" r:id="rId7" display="https://www.digikey.com/product-detail/en/on-semiconductor/MC74VHC1G07DTT1G/MC74VHC1G07DTT1GOSCT-ND/1967117" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G34" r:id="rId8" display="https://www.digikey.com/product-detail/en/texas-instruments/SN74LVC1G06DBVR/296-8483-1-ND/377451" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G37" r:id="rId9" display="https://www.digikey.com/product-detail/en/texas-instruments/BQ24650RVAT/296-27699-1-ND/2352706" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G38" r:id="rId10" display="https://www.digikey.com/product-detail/en/texas-instruments/BQ28Z610DRZT/296-43394-1-ND/5813465" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G39" r:id="rId11" display="https://www.digikey.com/product-detail/en/diodes-incorporated/DMN6040SSD-13/DMN6040SSD-13DICT-ND/3481122" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G40" r:id="rId12" display="https://www.digikey.com/product-detail/en/diodes-incorporated/DMP4047SSD-13/DMP4047SSD-13DICT-ND/5147416" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G43" r:id="rId13" display="https://www.digikey.com/product-detail/en/molex-llc/0705450072/WM14782-ND/3302409" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G44" r:id="rId14" display="https://www.digikey.com/product-detail/en/molex-connector-corporation/0705450003/WM4186-ND/455677" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G42" r:id="rId15" display="https://www.digikey.com/product-detail/en/molex-connector-corporation/0705450049/WM14780-ND/3302397" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G45" r:id="rId16" display="https://www.digikey.com/product-detail/en/diodes-incorporated/LMV358SG-13/LMV358SG-13DICT-ND/2182572" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G46" r:id="rId17" display="https://www.digikey.com/product-detail/en/microchip-technology/MIC5219-3.3YM5-TR/576-1281-1-ND/771902" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G47" r:id="rId18" display="https://www.digikey.com/product-detail/en/mill-max-manufacturing-corp/310-43-163-41-105000/ED4164-63-ND/4455145" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G48" r:id="rId19" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/S2B-XH-A-LF-SN/455-2257-ND/1651055" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G50" r:id="rId20" display="https://www.digikey.com/product-detail/en/nexperia-usa-inc/PMEG4020ETP115/1727-1730-1-ND/4581267" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G51" r:id="rId21" display="https://www.digikey.com/product-detail/en/stmicroelectronics/STWD100NYWY3F/497-10058-1-ND/2175107" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G52" r:id="rId22" display="https://www.digikey.com/product-detail/en/texas-instruments/TCA9543ADR/296-42064-1-ND/5246241" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G53" r:id="rId23" display="https://www.digikey.com/product-detail/en/stmicroelectronics/TS7211AILT/497-3046-1-ND/634884" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G55" r:id="rId24" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/173950378/732-8242-5-ND/5725366" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G54" r:id="rId25" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/173950578/732-8243-5-ND/5725367" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G6" r:id="rId26" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-07100RL/311-100HRCT-ND/729835" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G9" r:id="rId27" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-0710ML/311-10.0MHRCT-ND/729828" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G10" r:id="rId28" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-0710RL/311-10.0HRCT-ND/729826" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G15" r:id="rId29" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-0715KL/311-15.0KHRCT-ND/729900" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G20" r:id="rId30" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-07232KL/311-232KHRCT-ND/730019" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G21" r:id="rId31" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RMCF0603FT2R00/RMCF0603FT2R00CT-ND/6053160" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G25" r:id="rId32" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-07300KL/311-300KHRCT-ND/730092" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G31" r:id="rId33" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-075K1L/311-5.10KHRCT-ND/730215" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G32" r:id="rId34" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RMCF0603FT4R99/RMCF0603FT4R99CT-ND/2418080" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="G35" r:id="rId35" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-0775KL/311-75.0KHRCT-ND/730325" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="G11" r:id="rId36" display="https://www.digikey.com/product-detail/en/yageo/RC1206FR-0710RL/311-10.0FRCT-ND/731429" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="G27" r:id="rId37" display="https://www.digikey.com/product-detail/en/yageo/PE2512FKE070R04L/YAG2155CT-ND/5139603" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="G23" r:id="rId38" display="https://www.digikey.com/product-detail/en/yageo/PA2512FKF070R002E/YAG2137CT-ND/5139585" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="G30" r:id="rId39" display="https://www.digikey.com/product-detail/en/yageo/CC1210KKX5R9BB475/311-3533-1-ND/7164554" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="G12" r:id="rId40" display="https://www.digikey.com/product-detail/en/yageo/CC1210ZKY5VGBB106/311-3546-1-ND/7164567" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="G28" r:id="rId41" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10B471KB8NNNC/1276-1094-1-ND/3889180" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="G19" r:id="rId42" display="https://www.digikey.com/product-detail/en/avx-corporation/06035A220JAT2A/478-1167-1-ND/564199" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="G24" r:id="rId43" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10A225KL8NNNC/1276-6726-1-ND/5961585" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="G41" r:id="rId44" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150060GS75000/732-4971-1-ND/4489896" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="G49" r:id="rId45" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150060RS75000/732-4978-1-ND/4489899" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="G36" r:id="rId46" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150060BS75000/732-4966-1-ND/4489893" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId47"/>

</xml_diff>